<commit_message>
new pmbw no di run
</commit_message>
<xml_diff>
--- a/Output Files/Runs TO DO.xlsx
+++ b/Output Files/Runs TO DO.xlsx
@@ -372,7 +372,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,10 +433,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>